<commit_message>
re-build analysis for average purchase price after replacing value_counts with nunique method, to obtain the statistics per player ignoring duplicates.
</commit_message>
<xml_diff>
--- a/HeroesOfPymoli/3_Purchasing_Analysis_by_Gender.xlsx
+++ b/HeroesOfPymoli/3_Purchasing_Analysis_by_Gender.xlsx
@@ -414,7 +414,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>$3.20</t>
+          <t>$4.47</t>
         </is>
       </c>
     </row>
@@ -439,7 +439,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>$3.02</t>
+          <t>$4.07</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>$3.35</t>
+          <t>$4.56</t>
         </is>
       </c>
     </row>

</xml_diff>